<commit_message>
updated some highlighting in the spreadsheet.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-docker-cis-overlay.xlsx
+++ b/cms-ars-3.1-moderate-docker-cis-overlay.xlsx
@@ -5,18 +5,17 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-docker-cis-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3F639E-B486-4C45-B56F-DD430C9795A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F3D47611-E130-3946-9651-8D79A98B69D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67200" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-docker-cis" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1598" uniqueCount="1142">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1598" uniqueCount="1141">
   <si>
     <t>title</t>
   </si>
@@ -11090,30 +11089,6 @@
     <t>Associated with M-1.4.rb_old. Trying to figure out what this is and if it can be removed.</t>
   </si>
   <si>
-    <r>
-      <t>["AC-3</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (3)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "4"]</t>
-    </r>
-  </si>
-  <si>
     <t>Associated with M-6.3.rb_old. Trying to figure out what this is and if it can be removed.</t>
   </si>
   <si>
@@ -11148,7 +11123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -11287,12 +11262,6 @@
       <strike/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -12018,8 +11987,8 @@
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13320,7 +13289,7 @@
       <c r="J25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="5" t="s">
         <v>1133</v>
       </c>
       <c r="L25" s="1" t="s">
@@ -13691,7 +13660,7 @@
       <c r="J32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="5" t="s">
         <v>1133</v>
       </c>
       <c r="L32" s="1" t="s">
@@ -14012,7 +13981,7 @@
       <c r="J38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K38" s="5" t="s">
         <v>1133</v>
       </c>
       <c r="L38" s="1" t="s">
@@ -15430,7 +15399,7 @@
         <v>41</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>689</v>
@@ -15746,7 +15715,7 @@
         <v>1</v>
       </c>
       <c r="T71" s="5" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="409.6">
@@ -17212,7 +17181,7 @@
         <v>1032</v>
       </c>
       <c r="T99" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="100" spans="1:20" ht="409.6">
@@ -17343,8 +17312,8 @@
       <c r="J102" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K102" s="1" t="s">
-        <v>1141</v>
+      <c r="K102" s="5" t="s">
+        <v>1140</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>1057</v>

</xml_diff>